<commit_message>
updated dataset 06142019 3pm
</commit_message>
<xml_diff>
--- a/coffeebyage.xlsx
+++ b/coffeebyage.xlsx
@@ -112,9 +112,6 @@
     <t>Coffee drinking U.S. consumers by age group 2018</t>
   </si>
   <si>
-    <t>Share of coffee drinkers</t>
-  </si>
-  <si>
     <t>18 to 24 years</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Age Group</t>
+  </si>
+  <si>
+    <t>Percent</t>
   </si>
 </sst>
 </file>
@@ -718,9 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -730,15 +728,15 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="7">
         <v>48</v>
@@ -747,7 +745,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7">
         <v>63</v>
@@ -756,7 +754,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7">
         <v>66</v>
@@ -765,7 +763,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="7">
         <v>72</v>

</xml_diff>